<commit_message>
Add DB and dataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\QACollaborationFinal\QACollaborationFinal\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\qacollaborationGithub\qacollaboration\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902C0776-6F62-4E7A-B83F-0632FCBAD212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC7A4A0-28A0-441C-B12F-FC2F91C506DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31710" yWindow="1470" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>testname</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>106.0</t>
+  </si>
+  <si>
+    <t>112.0</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +553,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>

</xml_diff>